<commit_message>
Changes to Test Framework
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -19,18 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>WorkflowFile</t>
   </si>
   <si>
-    <t>Success</t>
-  </si>
-  <si>
     <t>Number of Runs</t>
-  </si>
-  <si>
-    <t>Expected result of test</t>
   </si>
   <si>
     <t>Test_Framework\Tests\_wbTest_Example1.xaml</t>
@@ -360,45 +354,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="41.88671875" customWidth="1"/>
+    <col min="1" max="2" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C9" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Success,BRE,AppEx"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Test results now use format testNumer_+testNumber.ToString+workflowName+now
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -354,15 +354,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="57.7109375" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -379,6 +380,14 @@
       </c>
       <c r="B2">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented feature: Test Framework now also provides statistics of test runs.
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -1,8 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557D99F8-2BE8-4FC7-87D4-7A87E6B3277D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>WorkflowFile</t>
   </si>
@@ -28,6 +29,9 @@
   </si>
   <si>
     <t>Test_Framework\Tests\_wbTest_Example1.xaml</t>
+  </si>
+  <si>
+    <t>Test_Framework\Tests\_wbTest_Example2.xaml</t>
   </si>
 </sst>
 </file>
@@ -357,7 +361,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -379,15 +383,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug where MainTask's io_Audit argument was not initialized
</commit_message>
<xml_diff>
--- a/Test_Framework/_Tests.xlsx
+++ b/Test_Framework/_Tests.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27959DD-293F-45CF-8218-A476FB971F51}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3281081E-091D-448A-95A7-33010981CAB8}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -383,7 +383,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -391,7 +391,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>